<commit_message>
Tree building for families to be done on server
</commit_message>
<xml_diff>
--- a/auxillary/species_info.xlsx
+++ b/auxillary/species_info.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="2020" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Species for ChemoR Pipeline" sheetId="1" r:id="rId1"/>
+    <sheet name="species_info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,228 +27,315 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Clade</t>
+  </si>
+  <si>
+    <t>BioProject</t>
+  </si>
   <si>
     <t>ancylostoma_caninum</t>
   </si>
   <si>
+    <t>acani</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>Vb</t>
+  </si>
+  <si>
+    <t>PRJNA72585</t>
+  </si>
+  <si>
     <t>angiostrongylus_cantonensis</t>
   </si>
   <si>
+    <t>acant</t>
+  </si>
+  <si>
+    <t>Vd</t>
+  </si>
+  <si>
+    <t>PRJEB493</t>
+  </si>
+  <si>
     <t>ascaris_suum</t>
   </si>
   <si>
+    <t>asuum</t>
+  </si>
+  <si>
+    <t>IIIa</t>
+  </si>
+  <si>
+    <t>PRJNA80881</t>
+  </si>
+  <si>
     <t>brugia_malayi</t>
   </si>
   <si>
+    <t>bmala</t>
+  </si>
+  <si>
+    <t>IIIb</t>
+  </si>
+  <si>
+    <t>PRJNA10729</t>
+  </si>
+  <si>
     <t>caenorhabditis_elegans</t>
   </si>
   <si>
+    <t>celeg</t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
+    <t>PRJNA13758</t>
+  </si>
+  <si>
     <t>dictyocaulus_viviparus</t>
   </si>
   <si>
+    <t>dvivi</t>
+  </si>
+  <si>
+    <t>PRJNA72587</t>
+  </si>
+  <si>
     <t>dracunculus_medinensis</t>
   </si>
   <si>
+    <t>dmedi</t>
+  </si>
+  <si>
+    <t>PRJEB500</t>
+  </si>
+  <si>
     <t>haemonchus_contortus</t>
   </si>
   <si>
+    <t>hcont</t>
+  </si>
+  <si>
+    <t>Ve</t>
+  </si>
+  <si>
+    <t>PRJNA205202</t>
+  </si>
+  <si>
     <t>litomosoides_sigmodontis</t>
   </si>
   <si>
+    <t>lsigm</t>
+  </si>
+  <si>
+    <t>PRJEB3075</t>
+  </si>
+  <si>
     <t>loa_loa</t>
   </si>
   <si>
+    <t>lloa</t>
+  </si>
+  <si>
+    <t>PRJNA60051</t>
+  </si>
+  <si>
     <t>meloidogyne_hapla</t>
   </si>
   <si>
+    <t>mhapl</t>
+  </si>
+  <si>
+    <t>IVa</t>
+  </si>
+  <si>
+    <t>PRJNA29083</t>
+  </si>
+  <si>
     <t>necator_americanus</t>
   </si>
   <si>
+    <t>namer</t>
+  </si>
+  <si>
+    <t>PRJNA72135</t>
+  </si>
+  <si>
     <t>nippostrongylus_brasiliensis</t>
   </si>
   <si>
+    <t>nbras</t>
+  </si>
+  <si>
+    <t>PRJEB511</t>
+  </si>
+  <si>
     <t>onchocerca_volvulus</t>
   </si>
   <si>
+    <t>ovolv</t>
+  </si>
+  <si>
+    <t>PRJEB513</t>
+  </si>
+  <si>
     <t>panagrellus_redivivus</t>
   </si>
   <si>
+    <t>predi</t>
+  </si>
+  <si>
+    <t>PRJNA186477</t>
+  </si>
+  <si>
     <t>pristionchus_pacificus</t>
   </si>
   <si>
+    <t>ppaci</t>
+  </si>
+  <si>
+    <t>PRJNA12644</t>
+  </si>
+  <si>
     <t>rhabditophanes_kr3021</t>
   </si>
   <si>
+    <t>rkr30</t>
+  </si>
+  <si>
+    <t>IVb</t>
+  </si>
+  <si>
+    <t>PRJEB1297</t>
+  </si>
+  <si>
     <t>romanomermis_culicivorax</t>
   </si>
   <si>
+    <t>rculi</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>PRJEB1358</t>
+  </si>
+  <si>
     <t>strongyloides_ratti</t>
   </si>
   <si>
+    <t>sratt</t>
+  </si>
+  <si>
+    <t>PRJEB125</t>
+  </si>
+  <si>
     <t>syphacia_muris</t>
   </si>
   <si>
+    <t>smuri</t>
+  </si>
+  <si>
+    <t>PRJEB524</t>
+  </si>
+  <si>
     <t>thelazia_callipaeda</t>
   </si>
   <si>
+    <t>tcall</t>
+  </si>
+  <si>
+    <t>PRJEB1205</t>
+  </si>
+  <si>
     <t>toxocara_canis</t>
   </si>
   <si>
+    <t>tcani</t>
+  </si>
+  <si>
+    <t>PRJNA248777</t>
+  </si>
+  <si>
     <t>trichinella_spiralis</t>
   </si>
   <si>
+    <t>tspir</t>
+  </si>
+  <si>
+    <t>PRJNA257433</t>
+  </si>
+  <si>
     <t>trichuris_muris</t>
   </si>
   <si>
-    <t>gold</t>
+    <t>tmuri</t>
+  </si>
+  <si>
+    <t>PRJEB126</t>
   </si>
   <si>
     <t>onchocerca_ochengi</t>
   </si>
   <si>
+    <t>ooche</t>
+  </si>
+  <si>
+    <t>non-gold-filarid</t>
+  </si>
+  <si>
+    <t>PRJEB1809</t>
+  </si>
+  <si>
     <t>wuchereria_bancrofti</t>
   </si>
   <si>
+    <t>wbanc</t>
+  </si>
+  <si>
+    <t>PRJNA275548</t>
+  </si>
+  <si>
     <t>brugia_timori</t>
   </si>
   <si>
+    <t>btimo</t>
+  </si>
+  <si>
+    <t>PRJEB4663</t>
+  </si>
+  <si>
     <t>brugia_pahangi</t>
   </si>
   <si>
+    <t>bpaha</t>
+  </si>
+  <si>
+    <t>PRJEB497</t>
+  </si>
+  <si>
     <t>dirofilaria_immitis</t>
   </si>
   <si>
-    <t>non-gold-filarid</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Classification</t>
-  </si>
-  <si>
-    <t>Clade</t>
-  </si>
-  <si>
-    <t>rculi</t>
-  </si>
-  <si>
-    <t>tmuri</t>
-  </si>
-  <si>
-    <t>tspir</t>
-  </si>
-  <si>
-    <t>asuum</t>
-  </si>
-  <si>
-    <t>smuri</t>
-  </si>
-  <si>
-    <t>tcani</t>
-  </si>
-  <si>
-    <t>bmala</t>
-  </si>
-  <si>
-    <t>bpaha</t>
-  </si>
-  <si>
-    <t>btimo</t>
-  </si>
-  <si>
     <t>dimmi</t>
   </si>
   <si>
-    <t>lsigm</t>
-  </si>
-  <si>
-    <t>lloa</t>
-  </si>
-  <si>
-    <t>ooche</t>
-  </si>
-  <si>
-    <t>ovolv</t>
-  </si>
-  <si>
-    <t>tcall</t>
-  </si>
-  <si>
-    <t>wbanc</t>
-  </si>
-  <si>
-    <t>mhapl</t>
-  </si>
-  <si>
-    <t>rkr30</t>
-  </si>
-  <si>
-    <t>sratt</t>
-  </si>
-  <si>
-    <t>celeg</t>
-  </si>
-  <si>
-    <t>ppaci</t>
-  </si>
-  <si>
-    <t>acani</t>
-  </si>
-  <si>
-    <t>namer</t>
-  </si>
-  <si>
-    <t>acant</t>
-  </si>
-  <si>
-    <t>dvivi</t>
-  </si>
-  <si>
-    <t>hcont</t>
-  </si>
-  <si>
-    <t>nbras</t>
-  </si>
-  <si>
-    <t>dmedi</t>
-  </si>
-  <si>
-    <t>predi</t>
-  </si>
-  <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>IIIa</t>
-  </si>
-  <si>
-    <t>IIIb</t>
-  </si>
-  <si>
-    <t>IVa</t>
-  </si>
-  <si>
-    <t>IVb</t>
-  </si>
-  <si>
-    <t>Va</t>
-  </si>
-  <si>
-    <t>Vb</t>
-  </si>
-  <si>
-    <t>Vd</t>
-  </si>
-  <si>
-    <t>Ve</t>
-  </si>
-  <si>
-    <t>Genome Version</t>
+    <t>PRJEB1797</t>
   </si>
 </sst>
 </file>
@@ -566,443 +653,529 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>69</v>
+      <c r="E6" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="E19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="I2:I97">
-    <sortCondition ref="I2:I97"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>